<commit_message>
Added C3DC phs002431 testcases
</commit_message>
<xml_diff>
--- a/InputFiles/C3DC/TC03_C3DC_phs002431_Race-HispOrLatino.xlsx
+++ b/InputFiles/C3DC/TC03_C3DC_phs002431_Race-HispOrLatino.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-11-27-2024/Commons_Automation/InputFiles/C3DC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA5CC29-4EAF-DB40-BECB-263BE54FEA2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B188DDDC-640E-3245-937D-DD35EBA8ECA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-41500" yWindow="-1900" windowWidth="30240" windowHeight="24500" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -703,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -737,7 +737,7 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -771,7 +771,7 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="2"/>
@@ -780,7 +780,7 @@
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="2"/>

</xml_diff>